<commit_message>
Merging Mireias' BR with new sections by EST
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy-REGULATED-V2.0.2.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy-REGULATED-V2.0.2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="588" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -2668,7 +2668,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -47717,7 +47719,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW65"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -64457,7 +64461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW44"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -69956,7 +69962,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW23"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -72116,7 +72124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>